<commit_message>
UPDATE: read and inplementation of general script && TODO: fix errors on the process
</commit_message>
<xml_diff>
--- a/python-script-genesis/tabla_datos.xlsx
+++ b/python-script-genesis/tabla_datos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,45 +507,45 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>992576</v>
+        <v>155321</v>
       </c>
       <c r="B2" t="n">
-        <v>20723</v>
+        <v>22660</v>
       </c>
       <c r="C2" t="n">
-        <v>18764058658147</v>
+        <v>18764052604297</v>
       </c>
       <c r="D2" t="n">
-        <v>9684</v>
+        <v>9321</v>
       </c>
       <c r="E2" t="n">
-        <v>8300</v>
+        <v>6326</v>
       </c>
       <c r="F2" t="n">
-        <v>30000</v>
+        <v>25000</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>25/10/2023 12:00:00 a. m.</t>
+          <t>30/07/2023 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>25/10/2024 12:00:00 a. m.</t>
+          <t>30/07/2024 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1JM</t>
+          <t>FEB</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>02NC</t>
+          <t>04NC</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>271</v>
+        <v>430</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
@@ -555,51 +555,51 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>28/10/2023 1:02:04 p. m.</t>
+          <t>1/08/2023 9:00:11 a. m.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>992576</v>
+        <v>155321</v>
       </c>
       <c r="B3" t="n">
-        <v>20723</v>
+        <v>22660</v>
       </c>
       <c r="C3" t="n">
-        <v>18764038656784</v>
+        <v>18764032631242</v>
       </c>
       <c r="D3" t="n">
-        <v>8299</v>
+        <v>6353</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>30000</v>
+        <v>25000</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>28/10/2022 12:00:00 a. m.</t>
+          <t>4/08/2022 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>28/10/2023 12:00:00 a. m.</t>
+          <t>4/08/2023 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>1JM</t>
+          <t>FEB</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>02NC</t>
+          <t>04NC</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>248</v>
+        <v>388</v>
       </c>
       <c r="L3" t="n">
         <v>1</v>
@@ -609,51 +609,51 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2/12/2022 10:38:48 a. m.</t>
+          <t>4/08/2022 3:26:03 p. m.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>898004</v>
+        <v>155321</v>
       </c>
       <c r="B4" t="n">
-        <v>20723</v>
+        <v>22660</v>
       </c>
       <c r="C4" t="n">
-        <v>18764038656784</v>
+        <v>18764017506030</v>
       </c>
       <c r="D4" t="n">
-        <v>9</v>
+        <v>10001</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>5672</v>
       </c>
       <c r="F4" t="n">
-        <v>30000</v>
+        <v>10000</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>28/10/2022 12:00:00 a. m.</t>
+          <t>2/09/2021 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>28/10/2023 12:00:00 a. m.</t>
+          <t>2/09/2022 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>1JM</t>
+          <t>FEC4</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>02NC</t>
+          <t>04NC</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>1</v>
+        <v>261</v>
       </c>
       <c r="L4" t="n">
         <v>1</v>
@@ -661,107 +661,97 @@
       <c r="M4" t="n">
         <v>10000</v>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>1/12/2022 10:43:31 a. m.</t>
-        </is>
-      </c>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>898004</v>
+        <v>155321</v>
       </c>
       <c r="B5" t="n">
-        <v>20723</v>
+        <v>22660</v>
       </c>
       <c r="C5" t="n">
-        <v>18764038656784</v>
+        <v>18764003803351</v>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>5731</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>30000</v>
+        <v>10000</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>28/10/2022 12:00:00 a. m.</t>
+          <t>4/09/2020 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>28/10/2023 12:00:00 a. m.</t>
+          <t>4/09/2021 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>1JM</t>
+          <t>FEC4</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>03NC</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>133</v>
-      </c>
+          <t>04NC</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="n">
         <v>1</v>
       </c>
       <c r="M5" t="n">
         <v>10000</v>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>1/12/2022 10:16:08 a. m.</t>
-        </is>
-      </c>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>898697</v>
+        <v>899714</v>
       </c>
       <c r="B6" t="n">
-        <v>20723</v>
+        <v>22569</v>
       </c>
       <c r="C6" t="n">
-        <v>18764033355514</v>
+        <v>18764054147524</v>
       </c>
       <c r="D6" t="n">
-        <v>983</v>
+        <v>28368</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>25307</v>
       </c>
       <c r="F6" t="n">
-        <v>25000</v>
+        <v>30000</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>11/08/2022 12:00:00 a. m.</t>
+          <t>20/08/2023 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>11/08/2023 12:00:00 a. m.</t>
+          <t>20/08/2024 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>FEA</t>
+          <t>JAMC</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>03NC</t>
+          <t>2NC</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>133</v>
+        <v>624</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
@@ -771,63 +761,1003 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>19/08/2022 11:23:45 a. m.</t>
+          <t>23/08/2023 5:01:16 p. m.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>898697</v>
+        <v>899712</v>
       </c>
       <c r="B7" t="n">
-        <v>20723</v>
+        <v>22569</v>
       </c>
       <c r="C7" t="n">
-        <v>18764016262077</v>
+        <v>18764034805546</v>
       </c>
       <c r="D7" t="n">
-        <v>4655</v>
+        <v>25316</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>16551</v>
       </c>
       <c r="F7" t="n">
-        <v>10000</v>
+        <v>30000</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>11/08/2021 12:00:00 a. m.</t>
+          <t>28/08/2022 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>11/08/2022 12:00:00 a. m.</t>
+          <t>28/08/2023 12:00:00 a. m.</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>FEC4</t>
+          <t>JAMC</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>03NC</t>
+          <t>2NC</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>68</v>
+        <v>508</v>
       </c>
       <c r="L7" t="n">
         <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>10000</v>
+        <v>30000</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>31/07/2022 10:46:17 p. m.</t>
-        </is>
-      </c>
+          <t>30/08/2022 12:30:46 p. m.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>899712</v>
+      </c>
+      <c r="B8" t="n">
+        <v>22569</v>
+      </c>
+      <c r="C8" t="n">
+        <v>18764034805546</v>
+      </c>
+      <c r="D8" t="n">
+        <v>16576</v>
+      </c>
+      <c r="E8" t="n">
+        <v>16551</v>
+      </c>
+      <c r="F8" t="n">
+        <v>30000</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>28/08/2022 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>28/08/2023 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>JAMC</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>2NC</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>292</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" t="n">
+        <v>30000</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>30/08/2022 12:28:00 p. m.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>899714</v>
+      </c>
+      <c r="B9" t="n">
+        <v>22569</v>
+      </c>
+      <c r="C9" t="n">
+        <v>18764003893519</v>
+      </c>
+      <c r="D9" t="n">
+        <v>8261</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>30000</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>7/09/2020 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>7/09/2021 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>JAMC</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>2NC</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>124</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1</v>
+      </c>
+      <c r="M9" t="n">
+        <v>30000</v>
+      </c>
+      <c r="N9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>899712</v>
+      </c>
+      <c r="B10" t="n">
+        <v>22569</v>
+      </c>
+      <c r="C10" t="n">
+        <v>18764017337352</v>
+      </c>
+      <c r="D10" t="n">
+        <v>16576</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8260</v>
+      </c>
+      <c r="F10" t="n">
+        <v>30000</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>31/08/2021 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>31/08/2022 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>JAMC</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>2NC</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>292</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" t="n">
+        <v>30000</v>
+      </c>
+      <c r="N10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>843908</v>
+      </c>
+      <c r="B11" t="n">
+        <v>79104</v>
+      </c>
+      <c r="C11" t="n">
+        <v>18764056654984</v>
+      </c>
+      <c r="D11" t="n">
+        <v>20173</v>
+      </c>
+      <c r="E11" t="n">
+        <v>18586</v>
+      </c>
+      <c r="F11" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>24/09/2023 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>24/03/2024 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>FVE</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>00NC</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>3</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" t="n">
+        <v>10000</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>26/09/2023 5:00:57 p. m.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>843908</v>
+      </c>
+      <c r="B12" t="n">
+        <v>79104</v>
+      </c>
+      <c r="C12" t="n">
+        <v>18764046358763</v>
+      </c>
+      <c r="D12" t="n">
+        <v>18586</v>
+      </c>
+      <c r="E12" t="n">
+        <v>15474</v>
+      </c>
+      <c r="F12" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>23/03/2023 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>23/09/2023 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>FVE</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>00NC</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>2</v>
+      </c>
+      <c r="L12" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" t="n">
+        <v>10000</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>28/03/2023 1:58:10 p. m.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>843908</v>
+      </c>
+      <c r="B13" t="n">
+        <v>79104</v>
+      </c>
+      <c r="C13" t="n">
+        <v>18764036574801</v>
+      </c>
+      <c r="D13" t="n">
+        <v>15474</v>
+      </c>
+      <c r="E13" t="n">
+        <v>12250</v>
+      </c>
+      <c r="F13" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>22/09/2022 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>22/03/2023 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>FVE</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>00NC</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>2</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>23/09/2022 5:47:53 p. m.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>843908</v>
+      </c>
+      <c r="B14" t="n">
+        <v>79104</v>
+      </c>
+      <c r="C14" t="n">
+        <v>18764026966271</v>
+      </c>
+      <c r="D14" t="n">
+        <v>12192</v>
+      </c>
+      <c r="E14" t="n">
+        <v>9108</v>
+      </c>
+      <c r="F14" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>24/03/2022 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>24/09/2022 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>FVE</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>00NC</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" t="n">
+        <v>10000</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>25/03/2022 11:45:48 a. m.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>843908</v>
+      </c>
+      <c r="B15" t="n">
+        <v>79104</v>
+      </c>
+      <c r="C15" t="n">
+        <v>18764011782051</v>
+      </c>
+      <c r="D15" t="n">
+        <v>5753</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2360</v>
+      </c>
+      <c r="F15" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>24/03/2021 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>24/09/2021 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>FVE</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>00NC</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" t="n">
+        <v>10000</v>
+      </c>
+      <c r="N15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>843908</v>
+      </c>
+      <c r="B16" t="n">
+        <v>79104</v>
+      </c>
+      <c r="C16" t="n">
+        <v>18764004873192</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2458</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>29/09/2020 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>29/03/2021 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>FVE</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>00NC</t>
+        </is>
+      </c>
+      <c r="K16" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" t="n">
+        <v>10000</v>
+      </c>
+      <c r="N16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>843908</v>
+      </c>
+      <c r="B17" t="n">
+        <v>79104</v>
+      </c>
+      <c r="C17" t="n">
+        <v>18764018400758</v>
+      </c>
+      <c r="D17" t="n">
+        <v>9108</v>
+      </c>
+      <c r="E17" t="n">
+        <v>5750</v>
+      </c>
+      <c r="F17" t="n">
+        <v>40000</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>22/09/2021 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>22/03/2022 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>FVE</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>00NC</t>
+        </is>
+      </c>
+      <c r="K17" t="n">
+        <v>2</v>
+      </c>
+      <c r="L17" t="n">
+        <v>1</v>
+      </c>
+      <c r="M17" t="n">
+        <v>10000</v>
+      </c>
+      <c r="N17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>159613</v>
+      </c>
+      <c r="B18" t="n">
+        <v>62011</v>
+      </c>
+      <c r="C18" t="n">
+        <v>18764048530906</v>
+      </c>
+      <c r="D18" t="n">
+        <v>27307</v>
+      </c>
+      <c r="E18" t="n">
+        <v>20001</v>
+      </c>
+      <c r="F18" t="n">
+        <v>30000</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>4/05/2023 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>4/05/2024 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>03FE</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>01NC</t>
+        </is>
+      </c>
+      <c r="K18" t="n">
+        <v>1391</v>
+      </c>
+      <c r="L18" t="n">
+        <v>1</v>
+      </c>
+      <c r="M18" t="n">
+        <v>10000</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>5/05/2023 11:55:44 a. m.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>159613</v>
+      </c>
+      <c r="B19" t="n">
+        <v>62011</v>
+      </c>
+      <c r="C19" t="n">
+        <v>18764028593860</v>
+      </c>
+      <c r="D19" t="n">
+        <v>20001</v>
+      </c>
+      <c r="E19" t="n">
+        <v>10001</v>
+      </c>
+      <c r="F19" t="n">
+        <v>20000</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>5/05/2022 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>5/05/2023 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>03FE</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>01NC</t>
+        </is>
+      </c>
+      <c r="K19" t="n">
+        <v>531</v>
+      </c>
+      <c r="L19" t="n">
+        <v>1</v>
+      </c>
+      <c r="M19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>6/05/2022 10:12:29 a. m.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>159613</v>
+      </c>
+      <c r="B20" t="n">
+        <v>62011</v>
+      </c>
+      <c r="C20" t="n">
+        <v>18764018245128</v>
+      </c>
+      <c r="D20" t="n">
+        <v>10001</v>
+      </c>
+      <c r="E20" t="n">
+        <v>4763</v>
+      </c>
+      <c r="F20" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>17/09/2021 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>17/09/2022 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>03FE</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>01NC</t>
+        </is>
+      </c>
+      <c r="K20" t="n">
+        <v>265</v>
+      </c>
+      <c r="L20" t="n">
+        <v>1</v>
+      </c>
+      <c r="M20" t="n">
+        <v>10000</v>
+      </c>
+      <c r="N20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>159613</v>
+      </c>
+      <c r="B21" t="n">
+        <v>62011</v>
+      </c>
+      <c r="C21" t="n">
+        <v>18764004423626</v>
+      </c>
+      <c r="D21" t="n">
+        <v>4765</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>19/09/2020 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>19/09/2021 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>03FE</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>01NC</t>
+        </is>
+      </c>
+      <c r="K21" t="n">
+        <v>35</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1</v>
+      </c>
+      <c r="M21" t="n">
+        <v>10000</v>
+      </c>
+      <c r="N21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>991510</v>
+      </c>
+      <c r="B22" t="n">
+        <v>61822</v>
+      </c>
+      <c r="C22" t="n">
+        <v>18764061128505</v>
+      </c>
+      <c r="D22" t="n">
+        <v>24067</v>
+      </c>
+      <c r="E22" t="n">
+        <v>23670</v>
+      </c>
+      <c r="F22" t="n">
+        <v>30000</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2/12/2023 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>2/12/2024 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>FE1J</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>00NC</t>
+        </is>
+      </c>
+      <c r="K22" t="n">
+        <v>3829</v>
+      </c>
+      <c r="L22" t="n">
+        <v>1</v>
+      </c>
+      <c r="M22" t="n">
+        <v>10000</v>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>4/12/2023 7:01:27 a. m.</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>991510</v>
+      </c>
+      <c r="B23" t="n">
+        <v>61822</v>
+      </c>
+      <c r="C23" t="n">
+        <v>18764041009299</v>
+      </c>
+      <c r="D23" t="n">
+        <v>23668</v>
+      </c>
+      <c r="E23" t="n">
+        <v>14020</v>
+      </c>
+      <c r="F23" t="n">
+        <v>30000</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>9/12/2022 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>9/12/2023 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>FE1J</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>00NC</t>
+        </is>
+      </c>
+      <c r="K23" t="n">
+        <v>3819</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1</v>
+      </c>
+      <c r="M23" t="n">
+        <v>10000</v>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>10/12/2022 8:28:21 a. m.</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>991510</v>
+      </c>
+      <c r="B24" t="n">
+        <v>61822</v>
+      </c>
+      <c r="C24" t="n">
+        <v>18764022535446</v>
+      </c>
+      <c r="D24" t="n">
+        <v>14020</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1985</v>
+      </c>
+      <c r="F24" t="n">
+        <v>30000</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>9/12/2021 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>9/12/2022 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>FE1J</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>00NC</t>
+        </is>
+      </c>
+      <c r="K24" t="n">
+        <v>3643</v>
+      </c>
+      <c r="L24" t="n">
+        <v>1</v>
+      </c>
+      <c r="M24" t="n">
+        <v>10000</v>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>10/12/2021 11:13:53 a. m.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>991510</v>
+      </c>
+      <c r="B25" t="n">
+        <v>61822</v>
+      </c>
+      <c r="C25" t="n">
+        <v>18764008616549</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1985</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" t="n">
+        <v>30000</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>9/12/2020 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>9/12/2021 12:00:00 a. m.</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>FE1J</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>00NC</t>
+        </is>
+      </c>
+      <c r="K25" t="n">
+        <v>154</v>
+      </c>
+      <c r="L25" t="n">
+        <v>1</v>
+      </c>
+      <c r="M25" t="n">
+        <v>10000</v>
+      </c>
+      <c r="N25" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>